<commit_message>
ajustando provas de educação no campo
</commit_message>
<xml_diff>
--- a/educ_campo/gabarito.xlsx
+++ b/educ_campo/gabarito.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tassiovalle/Documents/optical-mark-recognizer/educ_campo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{934DF4B4-4E60-BC4D-A234-DF11CFE82E2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FCC7291-F3B6-E24A-84B1-07A2B78D6340}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3900" yWindow="2200" windowWidth="28040" windowHeight="17440" xr2:uid="{7C65DD22-FAF3-DF4A-B386-AD82B1BB38EB}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="6">
   <si>
     <t>Questão</t>
   </si>
@@ -45,6 +45,15 @@
   </si>
   <si>
     <t>C</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>B</t>
   </si>
 </sst>
 </file>
@@ -453,10 +462,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB5F38DD-4FAF-C046-857A-752CEAB51067}">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -477,7 +486,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -493,7 +502,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -501,7 +510,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -509,7 +518,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -517,7 +526,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -533,7 +542,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -541,7 +550,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -549,7 +558,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -557,7 +566,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -565,7 +574,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -581,7 +590,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
@@ -589,47 +598,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="2">
-        <v>16</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="2">
-        <v>17</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="2">
-        <v>18</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" s="2">
-        <v>19</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="2">
-        <v>20</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>